<commit_message>
added Math GPA section
</commit_message>
<xml_diff>
--- a/NYOI Data/2021 Member Survey Report.xlsx
+++ b/NYOI Data/2021 Member Survey Report.xlsx
@@ -24853,9 +24853,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A06437C5D36E4C4FAAFD3528C5BF3240" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0677823491e8161b34aa52b98ae31ec6">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819d11e8-b16f-487f-9179-05ebbfb67dc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a09e3566b60afb0f7fd46840ced6715" ns2:_="">
-    <xsd:import namespace="819d11e8-b16f-487f-9179-05ebbfb67dc7"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4024CF44A37F04291FF95658E7ECBDA" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48157437e3e8b05a4b43e78227dbda30">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84e1b615-c911-4e56-969f-e617c0ee68b8" xmlns:ns3="c5f4af1b-4ac5-4e1f-9de7-f6f66fd97f0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2bbc3cefdcb64ba40b13a96d645c71cb" ns2:_="" ns3:_="">
+    <xsd:import namespace="84e1b615-c911-4e56-969f-e617c0ee68b8"/>
+    <xsd:import namespace="c5f4af1b-4ac5-4e1f-9de7-f6f66fd97f0e"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -24864,6 +24865,18 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -24871,7 +24884,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="819d11e8-b16f-487f-9179-05ebbfb67dc7" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="84e1b615-c911-4e56-969f-e617c0ee68b8" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -24883,6 +24896,98 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a617ba4a-2656-4853-a117-80cdf3c5b071" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c5f4af1b-4ac5-4e1f-9de7-f6f66fd97f0e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{4f51db75-969f-4614-8e87-7d7bbf8477d9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="c5f4af1b-4ac5-4e1f-9de7-f6f66fd97f0e">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -24995,12 +25100,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="84e1b615-c911-4e56-969f-e617c0ee68b8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c5f4af1b-4ac5-4e1f-9de7-f6f66fd97f0e" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7DA9D4E-C3BC-4EB9-9898-37A7D0B0CB10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F43C5438-FE46-43FE-83F3-EFC733150765}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>